<commit_message>
haciendo estadisticas de pedidos
</commit_message>
<xml_diff>
--- a/tips tp.xlsx
+++ b/tips tp.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfernandez_mecon\Desktop\GitHub\comandaLab4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600"/>
   </bookViews>
@@ -69,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,12 +94,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -126,12 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,6 +139,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -189,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,7 +437,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +499,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="4"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -513,7 +514,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="4"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>